<commit_message>
Changes to the Dev notebook
</commit_message>
<xml_diff>
--- a/MLB/DailyPitcherModel/Pitcher-Tracker.xlsx
+++ b/MLB/DailyPitcherModel/Pitcher-Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-01-24" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,6 +11,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-07-24" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-09-24" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-10-24" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-11-24" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-12-24" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-13-24" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-16-24" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -20,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -65,6 +69,19 @@
       <b val="1"/>
       <sz val="12"/>
     </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -157,11 +174,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -180,11 +233,50 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4125,8 +4217,8 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -4238,7 +4330,9 @@
       <c r="I2" t="n">
         <v>10.18</v>
       </c>
-      <c r="J2" s="2" t="n"/>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K2">
         <f>COUNTIF(J:J, 1)</f>
         <v/>
@@ -4287,7 +4381,9 @@
       <c r="I3" t="n">
         <v>11</v>
       </c>
-      <c r="J3" s="2" t="n"/>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n"/>
       <c r="M3" s="2" t="n"/>
@@ -4328,7 +4424,9 @@
       <c r="I4" t="n">
         <v>11.78</v>
       </c>
-      <c r="J4" s="2" t="n"/>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K4" s="2" t="n"/>
       <c r="L4" s="2" t="n"/>
       <c r="M4" s="2" t="n"/>
@@ -4369,7 +4467,9 @@
       <c r="I5" t="n">
         <v>14.29</v>
       </c>
-      <c r="J5" s="2" t="n"/>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K5" s="2" t="n"/>
       <c r="L5" s="2" t="n"/>
       <c r="M5" s="2" t="n"/>
@@ -4451,7 +4551,9 @@
       <c r="I7" t="n">
         <v>18.4</v>
       </c>
-      <c r="J7" s="2" t="n"/>
+      <c r="J7" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K7" s="2" t="n"/>
       <c r="L7" s="2" t="n"/>
       <c r="M7" s="2" t="n"/>
@@ -4492,7 +4594,9 @@
       <c r="I8" t="n">
         <v>18.8</v>
       </c>
-      <c r="J8" s="2" t="n"/>
+      <c r="J8" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K8" s="2" t="n"/>
       <c r="L8" s="2" t="n"/>
       <c r="M8" s="2" t="n"/>
@@ -4533,7 +4637,9 @@
       <c r="I9" t="n">
         <v>19.8</v>
       </c>
-      <c r="J9" s="2" t="n"/>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" s="2" t="n"/>
       <c r="L9" s="2" t="n"/>
       <c r="M9" s="2" t="n"/>
@@ -4574,7 +4680,9 @@
       <c r="I10" t="n">
         <v>20</v>
       </c>
-      <c r="J10" s="2" t="n"/>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K10" s="2" t="n"/>
       <c r="L10" s="2" t="n"/>
       <c r="M10" s="2" t="n"/>
@@ -4615,7 +4723,9 @@
       <c r="I11" t="n">
         <v>21.33</v>
       </c>
-      <c r="J11" s="2" t="n"/>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K11" s="2" t="n"/>
       <c r="L11" s="2" t="n"/>
       <c r="M11" s="2" t="n"/>
@@ -4656,83 +4766,1210 @@
       <c r="I12" t="n">
         <v>33</v>
       </c>
+      <c r="J12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Simeon Woods Richardson</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>18</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="I13" t="n">
+        <v>33.43</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>23</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Nick Martinez</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="I14" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J14">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="13.33203125" customWidth="1" min="3" max="3"/>
+    <col width="19.1640625" customWidth="1" min="5" max="5"/>
+    <col width="18.1640625" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="8" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Max Meyer</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I2" t="n">
+        <v>54</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>David Festa</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="I3" t="n">
+        <v>49.75</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>24</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Keider Montero</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="I4" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bailey Falter</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="I5" t="n">
+        <v>29.67</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tyler Glasnow</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="I6" t="n">
+        <v>29.33</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Keider Montero</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="I7" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tanner Bibee</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>22</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I8" t="n">
+        <v>17.33</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>OAK</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chris Bassitt</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>23</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>16.67</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>14</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Merrill Kelly</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I10" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>26</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Luis Severino</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>22</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+    </row>
+    <row r="12">
       <c r="J12" s="2" t="n"/>
       <c r="K12" s="2" t="n"/>
       <c r="L12" s="2" t="n"/>
       <c r="M12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="J13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="J14" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J14">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="24.5" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="9" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="9" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LAA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bowden Francis</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="I2" t="n">
+        <v>34.75</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sonny Gray</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>6</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="H3" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="I3" t="n">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Brandon Pfaadt</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1.63</v>
+      </c>
+      <c r="I4" t="n">
+        <v>23.29</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TEX</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Brayan Bello</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>21</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="I5" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Brady Singer</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.5600000000000001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>17</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Blake Snell</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>11</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-1.52</v>
+      </c>
+      <c r="I7" t="n">
+        <v>20.27</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>CLE</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Simeon Woods Richardson</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>18</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Pitcher Strikeouts</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>standard</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="I13" t="n">
-        <v>33.43</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Shota Imanaga</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>STL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Andrew Abbott</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>23</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>MIL</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Nick Martinez</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.95</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Davis Daniel</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I10" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Taj Bradley</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>16</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="I11" t="n">
+        <v>15.27</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>23</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CHC</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ben Lively</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Earned Runs Allowed</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>standard</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
         <v>2.5</v>
       </c>
-      <c r="H14" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="I14" t="n">
-        <v>44.8</v>
+      <c r="H12" t="n">
+        <v>-0.38</v>
+      </c>
+      <c r="I12" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4743,4 +5980,671 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="18.5" customWidth="1" min="3" max="3"/>
+    <col width="15.1640625" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="9" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="9" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Carson Fulmer</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="I2" t="n">
+        <v>38.29</v>
+      </c>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>LAA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kevin Gausman</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="I3" t="n">
+        <v>37.6</v>
+      </c>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>27</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Trevor Rogers</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I4" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Yusei Kikuchi</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="J7" s="2" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="J9" s="2" t="n"/>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="J10" s="2" t="n"/>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="J11" s="2" t="n"/>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="10" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cal Quantrill</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1.97</v>
+      </c>
+      <c r="I3" t="n">
+        <v>28.14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Aaron Civale</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="I4" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Aaron Civale</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>23</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="I5" t="n">
+        <v>19.6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ryne Nelson</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="I6" t="n">
+        <v>19.4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Sean Manaea</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>23</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="I7" t="n">
+        <v>16.17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TEX</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Simeon Woods Richardson</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>19</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I8" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>KC</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Nick Martinez</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="I9" t="n">
+        <v>15.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lasso regression, neural network, VIF, and more
</commit_message>
<xml_diff>
--- a/MLB/DailyPitcherModel/Pitcher-Tracker.xlsx
+++ b/MLB/DailyPitcherModel/Pitcher-Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="600" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-01-24" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,6 +15,13 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-12-24" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-13-24" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-16-24" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-18-24" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-19-24" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-22-24" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-23-24" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-27-24" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-29-24" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="09-02-24" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -24,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -80,6 +87,11 @@
       <sz val="12"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -91,12 +103,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -214,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -242,11 +269,64 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1128,6 +1208,3463 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="10" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CWS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Framber Valdez</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="I2" t="n">
+        <v>79.33</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CHC</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bowden Francis</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="I3" t="n">
+        <v>49.56</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CHC</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bowden Francis</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="I4" t="n">
+        <v>33.56</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Jake Woodford</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="I5" t="n">
+        <v>29.78</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sonny Gray</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="I6" t="n">
+        <v>29.67</v>
+      </c>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>22</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>OAK</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Blake Snell</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2.49</v>
+      </c>
+      <c r="I7" t="n">
+        <v>29.29</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>21</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>JP Sears</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1.49</v>
+      </c>
+      <c r="I8" t="n">
+        <v>27.09</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BAL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kutter Crawford</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="I9" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>36</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>JP Sears</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>18</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Joe Musgrove</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I11" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Paul Blackburn</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="I12" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NYM</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Valente Bellozo</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="I13" t="n">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Brady Singer</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>24</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-0.43</v>
+      </c>
+      <c r="I14" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>25</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NYM</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Valente Bellozo</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-0.9399999999999999</v>
+      </c>
+      <c r="I15" t="n">
+        <v>17.09</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>34</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Colin Rea</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="I16" t="n">
+        <v>16</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>20</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>LAA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Charlie Morton</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>21</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>6</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.95</v>
+      </c>
+      <c r="I17" t="n">
+        <v>15.83</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Taijuan Walker</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>11</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="I18" t="n">
+        <v>15.14</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J12 J14:J18">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="15.33203125" customWidth="1" min="3" max="3"/>
+    <col width="18.1640625" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="10" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bryan Woo</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1.41</v>
+      </c>
+      <c r="I2" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Jonathan Cannon</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="I3" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>KC</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Carson Fulmer</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.6899999999999999</v>
+      </c>
+      <c r="I4" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tanner Houck</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>26.67</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Joe Boyle</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1.25</v>
+      </c>
+      <c r="I6" t="n">
+        <v>22.73</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BAL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>David Peterson</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>13</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I7" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Gavin Stone</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I8" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kevin Gausman</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I9" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="J10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="J11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="J12" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="J14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="J15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="J16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="J17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="J18" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J12 J14:J18">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="15.83203125" customWidth="1" min="3" max="3"/>
+    <col width="17.6640625" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="10" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Patrick Corbin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="I2" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Luis Severino</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>20</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cal Quantrill</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I4" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NYY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gavin Williams</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="I5" t="n">
+        <v>24</v>
+      </c>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Patrick Corbin</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>25</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BAL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Spencer Arrighetti</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>22</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="I7" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="J7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Osvaldo Bido</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="I8" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="J8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Nick Lodolo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.95</v>
+      </c>
+      <c r="I9" t="n">
+        <v>15.83</v>
+      </c>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.93</v>
+      </c>
+      <c r="I10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="J10" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J10">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="11" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cade Povich</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="I2" t="n">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>STL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>David Festa</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="I3" t="n">
+        <v>45.25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>21</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bobby Miller</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1.66</v>
+      </c>
+      <c r="I4" t="n">
+        <v>33.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cade Povich</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1.46</v>
+      </c>
+      <c r="I5" t="n">
+        <v>26.55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Andrew Abbott</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>25</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="I6" t="n">
+        <v>26.18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Luis Castillo</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>26</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="I7" t="n">
+        <v>24.67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>28</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Andre Pallante</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>12</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1.31</v>
+      </c>
+      <c r="I8" t="n">
+        <v>23.82</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ryne Nelson</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>19</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>JP Sears</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>25</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="I10" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>23</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Luis Castillo</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>26</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>7</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1.37</v>
+      </c>
+      <c r="I11" t="n">
+        <v>19.57</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AZ</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Brayan Bello</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="I12" t="n">
+        <v>18.44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LAA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chris Bassitt</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>16.67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>37</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jack Kochanowicz</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Pitching Outs</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-2.37</v>
+      </c>
+      <c r="I14" t="n">
+        <v>15.29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Paul Blackburn</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="I15" t="n">
+        <v>15.14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="11" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cooper Criswell</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="I2" t="n">
+        <v>62.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TEX</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Garrett Crochet</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>26</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Miles Mikolas</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>26</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I4" t="n">
+        <v>31.67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>STL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dylan Cease</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="I5" t="n">
+        <v>29.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CHC</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Jared Jones</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cole Irvin</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I7" t="n">
+        <v>21.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>26</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Justin Steele</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1.13</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Aaron Nola</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>26</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AZ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sean Manaea</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>25</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.47</v>
+      </c>
+      <c r="I10" t="n">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>34</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cole Irvin</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="I11" t="n">
+        <v>18.29</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>23</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jeffrey Springs</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-1.04</v>
+      </c>
+      <c r="I12" t="n">
+        <v>17.33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-1.01</v>
+      </c>
+      <c r="I13" t="n">
+        <v>16.83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="11" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Jack Kochanowicz</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="I2" t="n">
+        <v>68.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sonny Gray</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="I3" t="n">
+        <v>54.8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>20</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bowden Francis</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Hits Allowed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1.93</v>
+      </c>
+      <c r="I4" t="n">
+        <v>35.09</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>STL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Michael King</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>27.27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LAD</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cade Povich</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Bowden Francis</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="I7" t="n">
+        <v>21.27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NYM</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ryne Nelson</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>22</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CWS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Nathan Eovaldi</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>23</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.91</v>
+      </c>
+      <c r="I9" t="n">
+        <v>15.17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>BatterTeam</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>Starts</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>Stat</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Line</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I1" s="11" t="inlineStr">
+        <is>
+          <t>Edge%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CWS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Corbin Burnes</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Earned Runs Allowed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="I2" t="n">
+        <v>47.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Zack Littell</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Joe Musgrove</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1.05</v>
+      </c>
+      <c r="I4" t="n">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Osvaldo Bido</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TEX</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="I6" t="n">
+        <v>16.17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Justin Verlander</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pitcher Strikeouts</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="I7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -5990,8 +9527,8 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6103,7 +9640,9 @@
       <c r="I2" t="n">
         <v>38.29</v>
       </c>
-      <c r="J2" s="2" t="n"/>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K2">
         <f>COUNTIF(J:J, 1)</f>
         <v/>
@@ -6152,7 +9691,9 @@
       <c r="I3" t="n">
         <v>37.6</v>
       </c>
-      <c r="J3" s="2" t="n"/>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n"/>
       <c r="M3" s="2" t="n"/>
@@ -6193,7 +9734,9 @@
       <c r="I4" t="n">
         <v>24.4</v>
       </c>
-      <c r="J4" s="2" t="n"/>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="K4" s="2" t="n"/>
       <c r="L4" s="2" t="n"/>
       <c r="M4" s="2" t="n"/>
@@ -6293,13 +9836,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="22.6640625" customWidth="1" min="3" max="3"/>
+    <col width="17.6640625" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="inlineStr">
@@ -6347,6 +9894,26 @@
           <t>Edge%</t>
         </is>
       </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -6384,6 +9951,20 @@
       <c r="I2" t="n">
         <v>33.33</v>
       </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(J:J, 1)</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>COUNTA(J2:J1000)</f>
+        <v/>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -6421,6 +10002,12 @@
       <c r="I3" t="n">
         <v>28.14</v>
       </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -6458,6 +10045,10 @@
       <c r="I4" t="n">
         <v>23.5</v>
       </c>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -6495,6 +10086,12 @@
       <c r="I5" t="n">
         <v>19.6</v>
       </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -6532,6 +10129,12 @@
       <c r="I6" t="n">
         <v>19.4</v>
       </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -6569,6 +10172,9 @@
       <c r="I7" t="n">
         <v>16.17</v>
       </c>
+      <c r="J7" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -6606,6 +10212,9 @@
       <c r="I8" t="n">
         <v>16</v>
       </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -6643,8 +10252,16 @@
       <c r="I9" t="n">
         <v>15.2</v>
       </c>
+      <c r="J9" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J9">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Strikeouts">
+      <formula>NOT(ISERROR(SEARCH("Strikeouts",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>